<commit_message>
liz and aaron adding to paper
</commit_message>
<xml_diff>
--- a/data/UI_20200326_states.xlsx
+++ b/data/UI_20200326_states.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PSG24/Dropbox/GoogleTrendsUINowcast/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethpancotti/Documents/GitHub/GoogleTrendsUINowcast/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B005CA1E-23EF-424E-AB06-1265AD859A53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E3B58A-40B1-CF4E-9858-4A52131B364B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -618,19 +618,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="top" indent="2" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
@@ -638,11 +644,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -926,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46:H46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -938,19 +947,19 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="8"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -958,15 +967,15 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>9490</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3">
+      <c r="E2" s="2"/>
+      <c r="F2" s="9">
         <v>1819</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="3">
         <v>7671</v>
       </c>
@@ -978,15 +987,15 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>8225</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3">
+      <c r="E3" s="2"/>
+      <c r="F3" s="9">
         <v>1120</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="3">
         <v>7105</v>
       </c>
@@ -998,15 +1007,15 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <v>29268</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3">
+      <c r="E4" s="2"/>
+      <c r="F4" s="9">
         <v>3844</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="3">
         <v>25424</v>
       </c>
@@ -1018,15 +1027,15 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>8958</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="3">
+      <c r="E5" s="2"/>
+      <c r="F5" s="9">
         <v>1382</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="3">
         <v>7576</v>
       </c>
@@ -1038,15 +1047,15 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="2">
+      <c r="D6" s="6">
         <v>186809</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3">
+      <c r="E6" s="6"/>
+      <c r="F6" s="9">
         <v>57606</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="3">
         <v>129203</v>
       </c>
@@ -1058,15 +1067,15 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>19429</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="9">
         <v>2321</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="3">
         <v>17108</v>
       </c>
@@ -1078,15 +1087,15 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <v>25098</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="3">
+      <c r="E8" s="2"/>
+      <c r="F8" s="9">
         <v>3440</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
       <c r="I8" s="3">
         <v>21658</v>
       </c>
@@ -1098,15 +1107,15 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="4">
+      <c r="D9" s="2">
         <v>10720</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5">
+      <c r="E9" s="2"/>
+      <c r="F9" s="10">
         <v>472</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
       <c r="I9" s="3">
         <v>10248</v>
       </c>
@@ -1118,15 +1127,15 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="4">
+      <c r="D10" s="2">
         <v>13473</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="3">
+      <c r="E10" s="2"/>
+      <c r="F10" s="9">
         <v>1213</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
       <c r="I10" s="3">
         <v>12260</v>
       </c>
@@ -1138,15 +1147,15 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="4">
+      <c r="D11" s="2">
         <v>74021</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="3">
+      <c r="E11" s="2"/>
+      <c r="F11" s="9">
         <v>6463</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="3">
         <v>67558</v>
       </c>
@@ -1158,15 +1167,15 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="4">
+      <c r="D12" s="2">
         <v>11746</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3">
+      <c r="E12" s="2"/>
+      <c r="F12" s="9">
         <v>5445</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="3">
         <v>6301</v>
       </c>
@@ -1178,15 +1187,15 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="4">
+      <c r="D13" s="2">
         <v>8904</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3">
+      <c r="E13" s="2"/>
+      <c r="F13" s="9">
         <v>1589</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="3">
         <v>7315</v>
       </c>
@@ -1198,15 +1207,15 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="4">
+      <c r="D14" s="2">
         <v>13314</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3">
+      <c r="E14" s="2"/>
+      <c r="F14" s="9">
         <v>1031</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
       <c r="I14" s="3">
         <v>12283</v>
       </c>
@@ -1218,15 +1227,15 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="2">
+      <c r="D15" s="6">
         <v>114663</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3">
+      <c r="E15" s="6"/>
+      <c r="F15" s="9">
         <v>10870</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
       <c r="I15" s="3">
         <v>103793</v>
       </c>
@@ -1238,15 +1247,15 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="4">
+      <c r="D16" s="2">
         <v>61635</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="3">
+      <c r="E16" s="2"/>
+      <c r="F16" s="9">
         <v>2596</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
       <c r="I16" s="3">
         <v>59039</v>
       </c>
@@ -1258,15 +1267,15 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="4">
+      <c r="D17" s="2">
         <v>41890</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="3">
+      <c r="E17" s="2"/>
+      <c r="F17" s="9">
         <v>2229</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
       <c r="I17" s="3">
         <v>39661</v>
       </c>
@@ -1278,15 +1287,15 @@
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="4">
+      <c r="D18" s="2">
         <v>23687</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3">
+      <c r="E18" s="2"/>
+      <c r="F18" s="9">
         <v>1755</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
       <c r="I18" s="3">
         <v>21932</v>
       </c>
@@ -1298,15 +1307,15 @@
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="4">
+      <c r="D19" s="2">
         <v>48847</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="3">
+      <c r="E19" s="2"/>
+      <c r="F19" s="9">
         <v>2785</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
       <c r="I19" s="3">
         <v>46062</v>
       </c>
@@ -1318,15 +1327,15 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="4">
+      <c r="D20" s="2">
         <v>72620</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="3">
+      <c r="E20" s="2"/>
+      <c r="F20" s="9">
         <v>2255</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
       <c r="I20" s="3">
         <v>70365</v>
       </c>
@@ -1338,15 +1347,15 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="4">
+      <c r="D21" s="2">
         <v>21197</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="5">
+      <c r="E21" s="2"/>
+      <c r="F21" s="10">
         <v>634</v>
       </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
       <c r="I21" s="3">
         <v>20563</v>
       </c>
@@ -1358,15 +1367,15 @@
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="4">
+      <c r="D22" s="2">
         <v>41882</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="3">
+      <c r="E22" s="2"/>
+      <c r="F22" s="9">
         <v>3864</v>
       </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
       <c r="I22" s="3">
         <v>38018</v>
       </c>
@@ -1378,15 +1387,15 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="2">
+      <c r="D23" s="6">
         <v>147995</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3">
+      <c r="E23" s="6"/>
+      <c r="F23" s="9">
         <v>7449</v>
       </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
       <c r="I23" s="3">
         <v>140546</v>
       </c>
@@ -1398,15 +1407,15 @@
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="2">
+      <c r="D24" s="6">
         <v>129298</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3">
+      <c r="E24" s="6"/>
+      <c r="F24" s="9">
         <v>5338</v>
       </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
       <c r="I24" s="3">
         <v>123960</v>
       </c>
@@ -1418,15 +1427,15 @@
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="2">
+      <c r="D25" s="6">
         <v>116438</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="3">
+      <c r="E25" s="6"/>
+      <c r="F25" s="9">
         <v>4010</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
       <c r="I25" s="3">
         <v>112428</v>
       </c>
@@ -1438,15 +1447,15 @@
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="4">
+      <c r="D26" s="2">
         <v>6723</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3">
+      <c r="E26" s="2"/>
+      <c r="F26" s="9">
         <v>1147</v>
       </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
       <c r="I26" s="3">
         <v>5576</v>
       </c>
@@ -1458,15 +1467,15 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="4">
+      <c r="D27" s="2">
         <v>40508</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="3">
+      <c r="E27" s="2"/>
+      <c r="F27" s="9">
         <v>4016</v>
       </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
       <c r="I27" s="3">
         <v>36492</v>
       </c>
@@ -1478,15 +1487,15 @@
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="4">
+      <c r="D28" s="2">
         <v>14704</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="5">
+      <c r="E28" s="2"/>
+      <c r="F28" s="10">
         <v>817</v>
       </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
       <c r="I28" s="3">
         <v>13887</v>
       </c>
@@ -1498,15 +1507,15 @@
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="4">
+      <c r="D29" s="2">
         <v>15668</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="5">
+      <c r="E29" s="2"/>
+      <c r="F29" s="10">
         <v>795</v>
       </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
       <c r="I29" s="3">
         <v>14873</v>
       </c>
@@ -1518,15 +1527,15 @@
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="4">
+      <c r="D30" s="2">
         <v>93036</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="3">
+      <c r="E30" s="2"/>
+      <c r="F30" s="9">
         <v>6356</v>
       </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
       <c r="I30" s="3">
         <v>86680</v>
       </c>
@@ -1538,19 +1547,19 @@
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="4">
+      <c r="D31" s="2">
         <v>21878</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="5">
+      <c r="E31" s="2"/>
+      <c r="F31" s="10">
         <v>642</v>
       </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5">
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="7">
         <v>21236</v>
       </c>
-      <c r="J31" s="5"/>
+      <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
@@ -1558,15 +1567,15 @@
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="2">
+      <c r="D32" s="6">
         <v>155454</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="3">
+      <c r="E32" s="6"/>
+      <c r="F32" s="9">
         <v>9467</v>
       </c>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
       <c r="I32" s="3">
         <v>145987</v>
       </c>
@@ -1578,15 +1587,15 @@
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="4">
+      <c r="D33" s="2">
         <v>17187</v>
       </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="5">
+      <c r="E33" s="2"/>
+      <c r="F33" s="10">
         <v>869</v>
       </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
       <c r="I33" s="3">
         <v>16318</v>
       </c>
@@ -1598,15 +1607,15 @@
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="4">
+      <c r="D34" s="2">
         <v>80334</v>
       </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="3">
+      <c r="E34" s="2"/>
+      <c r="F34" s="9">
         <v>14272</v>
       </c>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
       <c r="I34" s="3">
         <v>66062</v>
       </c>
@@ -1618,15 +1627,15 @@
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="4">
+      <c r="D35" s="2">
         <v>93587</v>
       </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="3">
+      <c r="E35" s="2"/>
+      <c r="F35" s="9">
         <v>3533</v>
       </c>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
       <c r="I35" s="3">
         <v>90054</v>
       </c>
@@ -1638,35 +1647,35 @@
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="4">
+      <c r="D36" s="2">
         <v>5968</v>
       </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="5">
+      <c r="E36" s="2"/>
+      <c r="F36" s="10">
         <v>415</v>
       </c>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
       <c r="I36" s="3">
         <v>5553</v>
       </c>
       <c r="J36" s="3"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="2">
+      <c r="D37" s="6">
         <v>187784</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="3">
+      <c r="E37" s="6"/>
+      <c r="F37" s="9">
         <v>7046</v>
       </c>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
       <c r="I37" s="3">
         <v>180738</v>
       </c>
@@ -1678,15 +1687,15 @@
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="4">
+      <c r="D38" s="2">
         <v>17720</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="3">
+      <c r="E38" s="2"/>
+      <c r="F38" s="9">
         <v>1836</v>
       </c>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
       <c r="I38" s="3">
         <v>15884</v>
       </c>
@@ -1698,35 +1707,35 @@
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="4">
+      <c r="D39" s="2">
         <v>22824</v>
       </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="3">
+      <c r="E39" s="2"/>
+      <c r="F39" s="9">
         <v>4269</v>
       </c>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
       <c r="I39" s="3">
         <v>18555</v>
       </c>
       <c r="J39" s="3"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="2">
+      <c r="D40" s="6">
         <v>378908</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="3">
+      <c r="E40" s="6"/>
+      <c r="F40" s="9">
         <v>15439</v>
       </c>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
       <c r="I40" s="3">
         <v>363469</v>
       </c>
@@ -1738,15 +1747,15 @@
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="4">
+      <c r="D41" s="2">
         <v>35436</v>
       </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="3">
+      <c r="E41" s="2"/>
+      <c r="F41" s="9">
         <v>1108</v>
       </c>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
       <c r="I41" s="3">
         <v>34328</v>
       </c>
@@ -1758,15 +1767,15 @@
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="4">
+      <c r="D42" s="2">
         <v>31064</v>
       </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="3">
+      <c r="E42" s="2"/>
+      <c r="F42" s="9">
         <v>2093</v>
       </c>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
       <c r="I42" s="3">
         <v>28971</v>
       </c>
@@ -1778,19 +1787,19 @@
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="4">
+      <c r="D43" s="2">
         <v>1703</v>
       </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="5">
+      <c r="E43" s="2"/>
+      <c r="F43" s="10">
         <v>190</v>
       </c>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5">
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="7">
         <v>1513</v>
       </c>
-      <c r="J43" s="5"/>
+      <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
@@ -1798,15 +1807,15 @@
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="4">
+      <c r="D44" s="2">
         <v>39096</v>
       </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="3">
+      <c r="E44" s="2"/>
+      <c r="F44" s="9">
         <v>2702</v>
       </c>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
       <c r="I44" s="3">
         <v>36394</v>
       </c>
@@ -1818,15 +1827,15 @@
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="2">
+      <c r="D45" s="6">
         <v>155657</v>
       </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="3">
+      <c r="E45" s="6"/>
+      <c r="F45" s="9">
         <v>16176</v>
       </c>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
       <c r="I45" s="3">
         <v>139481</v>
       </c>
@@ -1838,19 +1847,19 @@
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="4">
+      <c r="D46" s="2">
         <v>1314</v>
       </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="3">
+      <c r="E46" s="2"/>
+      <c r="F46" s="9">
         <v>1305</v>
       </c>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="5">
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="7">
         <v>9</v>
       </c>
-      <c r="J46" s="5"/>
+      <c r="J46" s="7"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
@@ -1858,15 +1867,15 @@
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="4">
+      <c r="D47" s="2">
         <v>3667</v>
       </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="5">
+      <c r="E47" s="2"/>
+      <c r="F47" s="10">
         <v>659</v>
       </c>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
       <c r="I47" s="3">
         <v>3008</v>
       </c>
@@ -1878,15 +1887,15 @@
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="4">
+      <c r="D48" s="2">
         <v>46885</v>
       </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="3">
+      <c r="E48" s="2"/>
+      <c r="F48" s="9">
         <v>2706</v>
       </c>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
       <c r="I48" s="3">
         <v>44179</v>
       </c>
@@ -1898,15 +1907,15 @@
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="2">
+      <c r="D49" s="6">
         <v>133478</v>
       </c>
-      <c r="E49" s="2"/>
-      <c r="F49" s="3">
+      <c r="E49" s="6"/>
+      <c r="F49" s="9">
         <v>14240</v>
       </c>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
       <c r="I49" s="3">
         <v>119238</v>
       </c>
@@ -1918,15 +1927,15 @@
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="4">
+      <c r="D50" s="2">
         <v>3435</v>
       </c>
-      <c r="E50" s="4"/>
-      <c r="F50" s="5">
+      <c r="E50" s="2"/>
+      <c r="F50" s="10">
         <v>865</v>
       </c>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
       <c r="I50" s="3">
         <v>2570</v>
       </c>
@@ -1938,15 +1947,15 @@
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="4">
+      <c r="D51" s="2">
         <v>50957</v>
       </c>
-      <c r="E51" s="4"/>
-      <c r="F51" s="3">
+      <c r="E51" s="2"/>
+      <c r="F51" s="9">
         <v>5190</v>
       </c>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
       <c r="I51" s="3">
         <v>45767</v>
       </c>
@@ -1958,230 +1967,178 @@
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="4">
+      <c r="D52" s="2">
         <v>2339</v>
       </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="5">
+      <c r="E52" s="2"/>
+      <c r="F52" s="10">
         <v>517</v>
       </c>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
       <c r="I52" s="3">
         <v>1822</v>
       </c>
       <c r="J52" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="208">
+  <mergeCells count="156">
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="I6:J6"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="I52:J52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>